<commit_message>
Added mising thrower bonuses. Reran notebooks.
</commit_message>
<xml_diff>
--- a/data/2021-12-29_DespotsGame_UnitStats.xlsx
+++ b/data/2021-12-29_DespotsGame_UnitStats.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="29">
   <si>
     <t xml:space="preserve">Level_1</t>
   </si>
@@ -1307,7 +1307,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.71"/>
@@ -1616,7 +1616,7 @@
       <selection pane="topLeft" activeCell="T37" activeCellId="0" sqref="T37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.71"/>
@@ -1943,7 +1943,7 @@
       <selection pane="topLeft" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.71"/>
@@ -2272,7 +2272,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.71"/>
@@ -2601,7 +2601,7 @@
       <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.71"/>
@@ -2927,10 +2927,10 @@
   <dimension ref="A1:Z991"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D81" activeCellId="0" sqref="D81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="49" t="s">
@@ -5849,10 +5849,18 @@
       <c r="Z81" s="50"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="50"/>
-      <c r="B82" s="50"/>
-      <c r="C82" s="50"/>
-      <c r="D82" s="50"/>
+      <c r="A82" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="B82" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>8</v>
+      </c>
       <c r="E82" s="50"/>
       <c r="F82" s="50"/>
       <c r="G82" s="50"/>
@@ -5877,10 +5885,18 @@
       <c r="Z82" s="50"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="50"/>
-      <c r="B83" s="50"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="50"/>
+      <c r="A83" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="B83" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D83" s="51" t="n">
+        <v>7</v>
+      </c>
       <c r="E83" s="50"/>
       <c r="F83" s="50"/>
       <c r="G83" s="50"/>
@@ -5905,10 +5921,18 @@
       <c r="Z83" s="50"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="50"/>
-      <c r="B84" s="50"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="50"/>
+      <c r="A84" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="B84" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" s="51" t="n">
+        <v>10</v>
+      </c>
       <c r="E84" s="50"/>
       <c r="F84" s="50"/>
       <c r="G84" s="50"/>
@@ -5933,10 +5957,18 @@
       <c r="Z84" s="50"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="50"/>
-      <c r="B85" s="50"/>
-      <c r="C85" s="50"/>
-      <c r="D85" s="50"/>
+      <c r="A85" s="51" t="n">
+        <v>2</v>
+      </c>
+      <c r="B85" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C85" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D85" s="51" t="n">
+        <v>7</v>
+      </c>
       <c r="E85" s="50"/>
       <c r="F85" s="50"/>
       <c r="G85" s="50"/>
@@ -5961,10 +5993,18 @@
       <c r="Z85" s="50"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="50"/>
-      <c r="B86" s="50"/>
-      <c r="C86" s="50"/>
-      <c r="D86" s="50"/>
+      <c r="A86" s="51" t="n">
+        <v>3</v>
+      </c>
+      <c r="B86" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C86" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" s="51" t="n">
+        <v>2</v>
+      </c>
       <c r="E86" s="50"/>
       <c r="F86" s="50"/>
       <c r="G86" s="50"/>
@@ -5989,10 +6029,18 @@
       <c r="Z86" s="50"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="50"/>
-      <c r="B87" s="50"/>
-      <c r="C87" s="50"/>
-      <c r="D87" s="50"/>
+      <c r="A87" s="51" t="n">
+        <v>3</v>
+      </c>
+      <c r="B87" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C87" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="51" t="n">
+        <v>10</v>
+      </c>
       <c r="E87" s="50"/>
       <c r="F87" s="50"/>
       <c r="G87" s="50"/>
@@ -6017,10 +6065,18 @@
       <c r="Z87" s="50"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="50"/>
-      <c r="B88" s="50"/>
-      <c r="C88" s="50"/>
-      <c r="D88" s="50"/>
+      <c r="A88" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="B88" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C88" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="51" t="n">
+        <v>5</v>
+      </c>
       <c r="E88" s="50"/>
       <c r="F88" s="50"/>
       <c r="G88" s="50"/>
@@ -6045,10 +6101,18 @@
       <c r="Z88" s="50"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="50"/>
-      <c r="B89" s="50"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="50"/>
+      <c r="A89" s="51" t="n">
+        <v>4</v>
+      </c>
+      <c r="B89" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C89" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="51" t="n">
+        <v>7</v>
+      </c>
       <c r="E89" s="50"/>
       <c r="F89" s="50"/>
       <c r="G89" s="50"/>
@@ -6073,10 +6137,18 @@
       <c r="Z89" s="50"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="50"/>
-      <c r="B90" s="50"/>
-      <c r="C90" s="50"/>
-      <c r="D90" s="50"/>
+      <c r="A90" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="B90" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="51" t="n">
+        <v>7</v>
+      </c>
       <c r="E90" s="50"/>
       <c r="F90" s="50"/>
       <c r="G90" s="50"/>
@@ -6101,10 +6173,18 @@
       <c r="Z90" s="50"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="50"/>
-      <c r="B91" s="50"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50"/>
+      <c r="A91" s="51" t="n">
+        <v>5</v>
+      </c>
+      <c r="B91" s="51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C91" s="50" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="51" t="n">
+        <v>7</v>
+      </c>
       <c r="E91" s="50"/>
       <c r="F91" s="50"/>
       <c r="G91" s="50"/>

</xml_diff>